<commit_message>
feat: (upload-service) validate notes sheet header row structure
</commit_message>
<xml_diff>
--- a/download.xlsx
+++ b/download.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="1" state="visible" r:id="rId2"/>
@@ -1107,13 +1107,13 @@
   </sheetPr>
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1379,11 +1379,11 @@
   </sheetPr>
   <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>